<commit_message>
Added average insert time.
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -8,106 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lescheng/Documents/notes/datafeeds/subscriptioncache/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77EB6F16-828C-C045-9690-E3A23CB25716}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75940424-F39A-F54E-B22D-C2A0D6827936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{0CE58859-4F50-D04F-B30D-5303C239E830}"/>
+    <workbookView xWindow="0" yWindow="-28340" windowWidth="68800" windowHeight="28340" xr2:uid="{0CE58859-4F50-D04F-B30D-5303C239E830}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="multimaps" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$107</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$108</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$111:$H$111</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$112:$H$112</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$109</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$A$107:$A$112</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$B$107:$B$112</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$C$107:$C$112</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$D$107:$D$112</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$E$107:$E$112</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$F$107:$F$112</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$110</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$G$107:$G$112</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$H$107:$H$112</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$111</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$A$2</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$A$5</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$A$6</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$B$2:$H$2</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Sheet1!$B$6:$H$6</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$112</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Sheet1!$A$2</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$A$5</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$A$6</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$B$2:$H$2</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$B$6:$H$6</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$107:$H$107</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">Sheet1!$A$2</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">Sheet1!$A$5</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">Sheet1!$A$6</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">Sheet1!$B$2:$H$2</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">Sheet1!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">Sheet1!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">Sheet1!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">Sheet1!$B$6:$H$6</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$108:$H$108</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">Sheet1!$A$2</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">Sheet1!$A$5</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">Sheet1!$A$6</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">Sheet1!$B$2:$H$2</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">Sheet1!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">Sheet1!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">Sheet1!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">Sheet1!$B$6:$H$6</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$109:$H$109</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">Sheet1!$A$2</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">Sheet1!$A$5</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">Sheet1!$A$6</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">Sheet1!$B$2:$H$2</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">Sheet1!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">Sheet1!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">Sheet1!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">Sheet1!$B$6:$H$6</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$110:$H$110</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">Sheet1!$A$107</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">Sheet1!$A$108</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">Sheet1!$A$109</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">Sheet1!$A$110</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">Sheet1!$A$111</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">Sheet1!$A$112</definedName>
-    <definedName name="_xlchart.v2.18" hidden="1">Sheet1!$B$107:$H$107</definedName>
-    <definedName name="_xlchart.v2.19" hidden="1">Sheet1!$B$108:$H$108</definedName>
-    <definedName name="_xlchart.v2.20" hidden="1">Sheet1!$B$109:$H$109</definedName>
-    <definedName name="_xlchart.v2.21" hidden="1">Sheet1!$B$110:$H$110</definedName>
-    <definedName name="_xlchart.v2.22" hidden="1">Sheet1!$B$111:$H$111</definedName>
-    <definedName name="_xlchart.v2.23" hidden="1">Sheet1!$B$112:$H$112</definedName>
-    <definedName name="_xlchart.v2.32" hidden="1">Sheet1!$A$107:$A$112</definedName>
-    <definedName name="_xlchart.v2.33" hidden="1">Sheet1!$B$107:$B$112</definedName>
-    <definedName name="_xlchart.v2.34" hidden="1">Sheet1!$C$107:$C$112</definedName>
-    <definedName name="_xlchart.v2.35" hidden="1">Sheet1!$D$107:$D$112</definedName>
-    <definedName name="_xlchart.v2.36" hidden="1">Sheet1!$E$107:$E$112</definedName>
-    <definedName name="_xlchart.v2.37" hidden="1">Sheet1!$F$107:$F$112</definedName>
-    <definedName name="_xlchart.v2.38" hidden="1">Sheet1!$G$107:$G$112</definedName>
-    <definedName name="_xlchart.v2.39" hidden="1">Sheet1!$H$107:$H$112</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -123,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="10">
   <si>
     <t>Database</t>
   </si>
@@ -150,6 +59,9 @@
   </si>
   <si>
     <t>Entries (min time to read a record from a map of n entries, ms)</t>
+  </si>
+  <si>
+    <t>Average insert time (ns)</t>
   </si>
 </sst>
 </file>
@@ -2612,6 +2524,843 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> insert time for maps of </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" i="1" baseline="0"/>
+              <a:t>n </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" i="0" baseline="0"/>
+              <a:t>size (ms)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ConcurrentMap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$9:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.0366650000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2123522E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8236340220000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3409416160000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6213738469999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4390021596E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0833141518999998E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E87A-BD4A-A61A-19B465565BB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Chronicle Map</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$10:$X$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9.6461959999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.21588732E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2261231811999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0230472701E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.03066373635E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1798504642600001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.193411938E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E87A-BD4A-A61A-19B465565BB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MapDB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$11:$X$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.1653236999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.31320953E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6089105199999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5514565905E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5633676071499999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7915305598199999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9498048713299999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E87A-BD4A-A61A-19B465565BB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LevelDB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$12:$X$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.1761083E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6440432799999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9773824088000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7883052823000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9251908054499998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9699290633800004E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7129083625799997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E87A-BD4A-A61A-19B465565BB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RocksDB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$8:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$13:$X$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.3353486999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.49668153E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5251296042E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5414504308E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5326223042999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6439728538799998E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0570654573399998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E87A-BD4A-A61A-19B465565BB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1721465743"/>
+        <c:axId val="1721467375"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1721465743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10000000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1721467375"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1721467375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1721465743"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2732,6 +3481,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3765,6 +4554,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4385,6 +5690,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>17561</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>175366</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>571086</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>185483</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E447455-237B-7846-8609-9B14D65739C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4690,22 +6031,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A870C54-8F60-324C-87C8-D285BA692A01}">
-  <dimension ref="A1:H221"/>
+  <dimension ref="A1:X221"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B217" sqref="B217:H221"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="18" max="18" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4730,8 +6073,11 @@
       <c r="H1" s="3">
         <v>10000000</v>
       </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4756,8 +6102,32 @@
       <c r="H2" s="2">
         <v>71558125855</v>
       </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="S2" s="2">
+        <v>10000</v>
+      </c>
+      <c r="T2" s="2">
+        <v>500000</v>
+      </c>
+      <c r="U2" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="V2" s="2">
+        <v>2000000</v>
+      </c>
+      <c r="W2" s="2">
+        <v>5000000</v>
+      </c>
+      <c r="X2" s="2">
+        <v>10000000</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -4782,8 +6152,32 @@
       <c r="H3" s="2">
         <v>119921207845</v>
       </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>5036.665</v>
+      </c>
+      <c r="S3">
+        <v>5212.3522000000003</v>
+      </c>
+      <c r="T3">
+        <v>5823.6340220000002</v>
+      </c>
+      <c r="U3">
+        <v>5340.9416160000001</v>
+      </c>
+      <c r="V3">
+        <v>6621.3738469999998</v>
+      </c>
+      <c r="W3">
+        <v>6439.0021595999997</v>
+      </c>
+      <c r="X3">
+        <v>7083.3141519000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4808,8 +6202,32 @@
       <c r="H4" s="2">
         <v>195563714485</v>
       </c>
+      <c r="Q4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>9646.1959999999999</v>
+      </c>
+      <c r="S4">
+        <v>12158.8732</v>
+      </c>
+      <c r="T4">
+        <v>12261.231812</v>
+      </c>
+      <c r="U4">
+        <v>10230.472701000001</v>
+      </c>
+      <c r="V4">
+        <v>10306.6373635</v>
+      </c>
+      <c r="W4">
+        <v>11798.504642600001</v>
+      </c>
+      <c r="X4">
+        <v>11934.11938</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4834,8 +6252,32 @@
       <c r="H5" s="2">
         <v>471899316407</v>
       </c>
+      <c r="Q5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>11653.236999999999</v>
+      </c>
+      <c r="S5">
+        <v>13132.095300000001</v>
+      </c>
+      <c r="T5">
+        <v>16089.1052</v>
+      </c>
+      <c r="U5">
+        <v>15514.565904999999</v>
+      </c>
+      <c r="V5">
+        <v>15633.6760715</v>
+      </c>
+      <c r="W5">
+        <v>17915.305598200001</v>
+      </c>
+      <c r="X5">
+        <v>19498.048713299999</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -4860,8 +6302,32 @@
       <c r="H6" s="2">
         <v>206313466401</v>
       </c>
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <v>11761.083000000001</v>
+      </c>
+      <c r="S6">
+        <v>16440.432799999999</v>
+      </c>
+      <c r="T6">
+        <v>19773.824088000001</v>
+      </c>
+      <c r="U6">
+        <v>27883.052823000002</v>
+      </c>
+      <c r="V6">
+        <v>29251.9080545</v>
+      </c>
+      <c r="W6">
+        <v>39699.290633800003</v>
+      </c>
+      <c r="X6">
+        <v>47129.083625799998</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>A1</f>
         <v>Database</v>
@@ -4894,8 +6360,32 @@
         <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
+      <c r="Q7" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <v>13353.486999999999</v>
+      </c>
+      <c r="S7">
+        <v>14966.8153</v>
+      </c>
+      <c r="T7">
+        <v>15251.296042</v>
+      </c>
+      <c r="U7">
+        <v>15414.504308</v>
+      </c>
+      <c r="V7">
+        <v>15326.223043</v>
+      </c>
+      <c r="W7">
+        <v>16439.728538799998</v>
+      </c>
+      <c r="X7">
+        <v>20570.654573399999</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f t="shared" ref="A8:A12" si="1">A2</f>
         <v>ConcurrentMap</v>
@@ -4928,8 +6418,32 @@
         <f t="shared" si="2"/>
         <v>71.558125855</v>
       </c>
+      <c r="Q8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1000</v>
+      </c>
+      <c r="S8" s="2">
+        <v>10000</v>
+      </c>
+      <c r="T8" s="2">
+        <v>500000</v>
+      </c>
+      <c r="U8" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="V8" s="2">
+        <v>2000000</v>
+      </c>
+      <c r="W8" s="2">
+        <v>5000000</v>
+      </c>
+      <c r="X8" s="2">
+        <v>10000000</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f t="shared" si="1"/>
         <v>Chronicle Map</v>
@@ -4962,8 +6476,39 @@
         <f t="shared" si="3"/>
         <v>119.921207845</v>
       </c>
+      <c r="Q9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <f>R3/(10^6)</f>
+        <v>5.0366650000000001E-3</v>
+      </c>
+      <c r="S9">
+        <f t="shared" ref="S9:X9" si="4">S3/(10^6)</f>
+        <v>5.2123522E-3</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="4"/>
+        <v>5.8236340220000002E-3</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="4"/>
+        <v>5.3409416160000002E-3</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="4"/>
+        <v>6.6213738469999995E-3</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="4"/>
+        <v>6.4390021596E-3</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="4"/>
+        <v>7.0833141518999998E-3</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f t="shared" si="1"/>
         <v>MapDB</v>
@@ -4996,8 +6541,39 @@
         <f t="shared" si="3"/>
         <v>195.56371448499999</v>
       </c>
+      <c r="Q10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R10">
+        <f t="shared" ref="R10:X10" si="5">R4/(10^6)</f>
+        <v>9.6461959999999992E-3</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="5"/>
+        <v>1.21588732E-2</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="5"/>
+        <v>1.2261231811999999E-2</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="5"/>
+        <v>1.0230472701E-2</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="5"/>
+        <v>1.03066373635E-2</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="5"/>
+        <v>1.1798504642600001E-2</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="5"/>
+        <v>1.193411938E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f t="shared" si="1"/>
         <v>LevelDB</v>
@@ -5030,8 +6606,39 @@
         <f t="shared" si="3"/>
         <v>471.89931640700001</v>
       </c>
+      <c r="Q11" t="s">
+        <v>3</v>
+      </c>
+      <c r="R11">
+        <f t="shared" ref="R11:X11" si="6">R5/(10^6)</f>
+        <v>1.1653236999999999E-2</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="6"/>
+        <v>1.31320953E-2</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="6"/>
+        <v>1.6089105199999999E-2</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="6"/>
+        <v>1.5514565905E-2</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="6"/>
+        <v>1.5633676071499999E-2</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="6"/>
+        <v>1.7915305598199999E-2</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="6"/>
+        <v>1.9498048713299999E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f t="shared" si="1"/>
         <v>RocksDB</v>
@@ -5063,6 +6670,70 @@
       <c r="H12">
         <f t="shared" si="3"/>
         <v>206.313466401</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>4</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ref="R12:X12" si="7">R6/(10^6)</f>
+        <v>1.1761083E-2</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="7"/>
+        <v>1.6440432799999998E-2</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="7"/>
+        <v>1.9773824088000002E-2</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="7"/>
+        <v>2.7883052823000003E-2</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="7"/>
+        <v>2.9251908054499998E-2</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="7"/>
+        <v>3.9699290633800004E-2</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="7"/>
+        <v>4.7129083625799997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Q13" t="s">
+        <v>5</v>
+      </c>
+      <c r="R13">
+        <f t="shared" ref="R13:X13" si="8">R7/(10^6)</f>
+        <v>1.3353486999999999E-2</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="8"/>
+        <v>1.49668153E-2</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="8"/>
+        <v>1.5251296042E-2</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="8"/>
+        <v>1.5414504308E-2</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="8"/>
+        <v>1.5326223042999999E-2</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="8"/>
+        <v>1.6439728538799998E-2</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="8"/>
+        <v>2.0570654573399998E-2</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -5201,37 +6872,37 @@
         <v>Database</v>
       </c>
       <c r="B59">
-        <f t="shared" ref="B59:H59" si="4">B54</f>
+        <f t="shared" ref="B59:H59" si="9">B54</f>
         <v>1000</v>
       </c>
       <c r="C59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10000</v>
       </c>
       <c r="D59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>500000</v>
       </c>
       <c r="E59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1000000</v>
       </c>
       <c r="F59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>2000000</v>
       </c>
       <c r="G59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5000000</v>
       </c>
       <c r="H59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10000000</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
-        <f t="shared" ref="A60:A63" si="5">A55</f>
+        <f t="shared" ref="A60:A63" si="10">A55</f>
         <v>Chronicle Map</v>
       </c>
       <c r="B60">
@@ -5239,7 +6910,7 @@
         <v>0.76185599999999998</v>
       </c>
       <c r="C60">
-        <f t="shared" ref="C60:G60" si="6">C55/(1000*1000)</f>
+        <f t="shared" ref="C60:G60" si="11">C55/(1000*1000)</f>
         <v>8.9251839999999998</v>
       </c>
       <c r="D60">
@@ -5247,15 +6918,15 @@
         <v>403.90246400000001</v>
       </c>
       <c r="E60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>807.80083200000001</v>
       </c>
       <c r="F60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1615.5975679999999</v>
       </c>
       <c r="G60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4003.0740479999999</v>
       </c>
       <c r="H60">
@@ -5265,103 +6936,103 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>MapDB</v>
       </c>
       <c r="B61">
-        <f t="shared" ref="B61:G63" si="7">B56/(1000*1000)</f>
+        <f t="shared" ref="B61:G63" si="12">B56/(1000*1000)</f>
         <v>2.0971519999999999</v>
       </c>
       <c r="C61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>8.3886079999999996</v>
       </c>
       <c r="D61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>346.03008</v>
       </c>
       <c r="E61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>684.72012800000005</v>
       </c>
       <c r="F61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1368.39168</v>
       </c>
       <c r="G61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>3448.7664639999998</v>
       </c>
       <c r="H61">
-        <f t="shared" ref="H61" si="8">H56/(1000*1000)</f>
+        <f t="shared" ref="H61" si="13">H56/(1000*1000)</f>
         <v>6974.0789759999998</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>LevelDB</v>
       </c>
       <c r="B62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.63625600000000004</v>
       </c>
       <c r="C62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>4.1776710000000001</v>
       </c>
       <c r="D62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>140.74940900000001</v>
       </c>
       <c r="E62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>281.787149</v>
       </c>
       <c r="F62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>561.65991699999995</v>
       </c>
       <c r="G62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1399.5495490000001</v>
       </c>
       <c r="H62">
-        <f t="shared" ref="H62" si="9">H57/(1000*1000)</f>
+        <f t="shared" ref="H62" si="14">H57/(1000*1000)</f>
         <v>2794.7321820000002</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>RocksDB</v>
       </c>
       <c r="B63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.66280300000000003</v>
       </c>
       <c r="C63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>6.3880160000000004</v>
       </c>
       <c r="D63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>173.85236900000001</v>
       </c>
       <c r="E63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>310.200853</v>
       </c>
       <c r="F63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>582.49709399999995</v>
       </c>
       <c r="G63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1445.2054659999999</v>
       </c>
       <c r="H63">
-        <f t="shared" ref="H63" si="10">H58/(1000*1000)</f>
+        <f t="shared" ref="H63" si="15">H58/(1000*1000)</f>
         <v>2809.9759370000002</v>
       </c>
     </row>
@@ -5527,37 +7198,37 @@
         <v>Database</v>
       </c>
       <c r="B107">
-        <f t="shared" ref="B107:H107" si="11">B101</f>
+        <f t="shared" ref="B107:H107" si="16">B101</f>
         <v>1000</v>
       </c>
       <c r="C107">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>10000</v>
       </c>
       <c r="D107">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>500000</v>
       </c>
       <c r="E107">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1000000</v>
       </c>
       <c r="F107">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2000000</v>
       </c>
       <c r="G107">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>5000000</v>
       </c>
       <c r="H107">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>10000000</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="str">
-        <f t="shared" ref="A108:A112" si="12">A102</f>
+        <f t="shared" ref="A108:A112" si="17">A102</f>
         <v>ConcurrentMap</v>
       </c>
       <c r="B108">
@@ -5565,163 +7236,163 @@
         <v>1.9941999999999998E-4</v>
       </c>
       <c r="C108">
-        <f t="shared" ref="C108:H108" si="13">C102/(10^6)</f>
+        <f t="shared" ref="C108:H108" si="18">C102/(10^6)</f>
         <v>2.5464999999999998E-4</v>
       </c>
       <c r="D108">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>3.4241000000000002E-4</v>
       </c>
       <c r="E108">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>3.7908000000000001E-4</v>
       </c>
       <c r="F108">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>3.9572000000000001E-4</v>
       </c>
       <c r="G108">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>4.6832999999999998E-4</v>
       </c>
       <c r="H108">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>4.9534999999999998E-4</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>Chronicle Map</v>
       </c>
       <c r="B109">
-        <f t="shared" ref="B109:H112" si="14">B103/(10^6)</f>
+        <f t="shared" ref="B109:H112" si="19">B103/(10^6)</f>
         <v>1.0818350000000001E-2</v>
       </c>
       <c r="C109">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.0673190000000001E-2</v>
       </c>
       <c r="D109">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.0831E-2</v>
       </c>
       <c r="E109">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.124467E-2</v>
       </c>
       <c r="F109">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.2809709999999998E-2</v>
       </c>
       <c r="G109">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.125525E-2</v>
       </c>
       <c r="H109">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.128501E-2</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>MapDB</v>
       </c>
       <c r="B110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.292395E-2</v>
       </c>
       <c r="C110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.28392E-2</v>
       </c>
       <c r="D110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.408188E-2</v>
       </c>
       <c r="E110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.2790459999999998E-2</v>
       </c>
       <c r="F110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.295316E-2</v>
       </c>
       <c r="G110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.347636E-2</v>
       </c>
       <c r="H110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.426855E-2</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>LevelDB</v>
       </c>
       <c r="B111">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.5955399999999999E-3</v>
       </c>
       <c r="C111">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>3.0793499999999998E-3</v>
       </c>
       <c r="D111">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>9.6693899999999999E-3</v>
       </c>
       <c r="E111">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>9.9954199999999997E-3</v>
       </c>
       <c r="F111">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.0494059999999999E-2</v>
       </c>
       <c r="G111">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.0708780000000001E-2</v>
       </c>
       <c r="H111">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>4.0025039999999998E-2</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>RocksDB</v>
       </c>
       <c r="B112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.3868299999999999E-3</v>
       </c>
       <c r="C112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.7440000000000001E-3</v>
       </c>
       <c r="D112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>1.499291E-2</v>
       </c>
       <c r="E112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>2.4813769999999999E-2</v>
       </c>
       <c r="F112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>3.8368480000000003E-2</v>
       </c>
       <c r="G112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>2.7162180000000001E-2</v>
       </c>
       <c r="H112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>4.4229900000000003E-2</v>
       </c>
     </row>
@@ -5892,147 +7563,147 @@
         <v>6.5399999999999996E-4</v>
       </c>
       <c r="C157">
-        <f t="shared" ref="C157:H157" si="15">C151/(10^6)</f>
+        <f t="shared" ref="C157:H157" si="20">C151/(10^6)</f>
         <v>9.9200000000000004E-4</v>
       </c>
       <c r="D157">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1.2335E-2</v>
       </c>
       <c r="E157">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1.9814999999999999E-2</v>
       </c>
       <c r="F157">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1.257E-2</v>
       </c>
       <c r="G157">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1.9401000000000002E-2</v>
       </c>
       <c r="H157">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0.13347400000000001</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B158">
-        <f t="shared" ref="B158:H161" si="16">B152/(10^6)</f>
+        <f t="shared" ref="B158:H161" si="21">B152/(10^6)</f>
         <v>8.5619000000000001E-2</v>
       </c>
       <c r="C158">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>3.9095999999999999E-2</v>
       </c>
       <c r="D158">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>90.166390000000007</v>
       </c>
       <c r="E158">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>179.99911399999999</v>
       </c>
       <c r="F158">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>3405.4899059999998</v>
       </c>
       <c r="G158">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>313.49678599999999</v>
       </c>
       <c r="H158">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>367.84904799999998</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B159">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>2.8681000000000002E-2</v>
       </c>
       <c r="C159">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>3.5869999999999999E-2</v>
       </c>
       <c r="D159">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>125.263621</v>
       </c>
       <c r="E159">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>85.507785999999996</v>
       </c>
       <c r="F159">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>126.82899999999999</v>
       </c>
       <c r="G159">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>468.82510200000002</v>
       </c>
       <c r="H159">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>336.43504000000001</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B160">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>1.5547E-2</v>
       </c>
       <c r="C160">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>2.4490000000000001E-2</v>
       </c>
       <c r="D160">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>4.7179010000000003</v>
       </c>
       <c r="E160">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>5.5538660000000002</v>
       </c>
       <c r="F160">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>8.4894029999999994</v>
       </c>
       <c r="G160">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>156.50303099999999</v>
       </c>
       <c r="H160">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>6287.5812930000002</v>
       </c>
     </row>
     <row r="161" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B161">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>1.5944E-2</v>
       </c>
       <c r="C161">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>1.5365E-2</v>
       </c>
       <c r="D161">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.10127899999999999</v>
       </c>
       <c r="E161">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.19653699999999999</v>
       </c>
       <c r="F161">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.18718899999999999</v>
       </c>
       <c r="G161">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.39402599999999999</v>
       </c>
       <c r="H161">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>288.44819000000001</v>
       </c>
     </row>
@@ -6203,147 +7874,147 @@
         <v>5.5000000000000002E-5</v>
       </c>
       <c r="C217">
-        <f t="shared" ref="C217:H217" si="17">C211/(10^6)</f>
+        <f t="shared" ref="C217:H217" si="22">C211/(10^6)</f>
         <v>4.8000000000000001E-5</v>
       </c>
       <c r="D217">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>4.5000000000000003E-5</v>
       </c>
       <c r="E217">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="F217">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="G217">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>5.8999999999999998E-5</v>
       </c>
       <c r="H217">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>5.7000000000000003E-5</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B218">
-        <f t="shared" ref="B218:H221" si="18">B212/(10^6)</f>
+        <f t="shared" ref="B218:H221" si="23">B212/(10^6)</f>
         <v>1.0208999999999999E-2</v>
       </c>
       <c r="C218">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.0255E-2</v>
       </c>
       <c r="D218">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.0057999999999999E-2</v>
       </c>
       <c r="E218">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>9.9360000000000004E-3</v>
       </c>
       <c r="F218">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>9.9369999999999997E-3</v>
       </c>
       <c r="G218">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>9.972E-3</v>
       </c>
       <c r="H218">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.0088E-2</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B219">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.1971000000000001E-2</v>
       </c>
       <c r="C219">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.2026E-2</v>
       </c>
       <c r="D219">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.2135999999999999E-2</v>
       </c>
       <c r="E219">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.0914E-2</v>
       </c>
       <c r="F219">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.0964E-2</v>
       </c>
       <c r="G219">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.1037E-2</v>
       </c>
       <c r="H219">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.1270000000000001E-2</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B220">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.0070000000000001E-3</v>
       </c>
       <c r="C220">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.106E-3</v>
       </c>
       <c r="D220">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.1349999999999999E-3</v>
       </c>
       <c r="E220">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>9.4899999999999997E-4</v>
       </c>
       <c r="F220">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.0039999999999999E-3</v>
       </c>
       <c r="G220">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>8.9899999999999995E-4</v>
       </c>
       <c r="H220">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>8.9400000000000005E-4</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B221">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>9.2299999999999999E-4</v>
       </c>
       <c r="C221">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.0480000000000001E-3</v>
       </c>
       <c r="D221">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.121E-3</v>
       </c>
       <c r="E221">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.1329999999999999E-3</v>
       </c>
       <c r="F221">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.147E-3</v>
       </c>
       <c r="G221">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.0120000000000001E-3</v>
       </c>
       <c r="H221">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1.1329999999999999E-3</v>
       </c>
     </row>
@@ -6352,4 +8023,151 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDA91B4-F9A5-934F-B58D-EC8583F2B90D}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C1" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D1" s="3">
+        <v>500000</v>
+      </c>
+      <c r="E1" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="F1" s="3">
+        <v>2000000</v>
+      </c>
+      <c r="G1" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="H1" s="3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>20292074</v>
+      </c>
+      <c r="C2" s="2">
+        <v>53030084</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2931994819</v>
+      </c>
+      <c r="E2" s="2">
+        <v>11762602746</v>
+      </c>
+      <c r="F2" s="2">
+        <v>13324460067</v>
+      </c>
+      <c r="G2" s="2">
+        <v>32402223087</v>
+      </c>
+      <c r="H2" s="2">
+        <v>71558125855</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>71871684</v>
+      </c>
+      <c r="C3" s="2">
+        <v>123063888</v>
+      </c>
+      <c r="D3" s="2">
+        <v>6155059112</v>
+      </c>
+      <c r="E3" s="2">
+        <v>22759969881</v>
+      </c>
+      <c r="F3" s="2">
+        <v>20722566561</v>
+      </c>
+      <c r="G3" s="2">
+        <v>59268268004</v>
+      </c>
+      <c r="H3" s="2">
+        <v>119921207845</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>23322210</v>
+      </c>
+      <c r="C4" s="2">
+        <v>132694232</v>
+      </c>
+      <c r="D4" s="2">
+        <v>8068651841</v>
+      </c>
+      <c r="E4" s="2">
+        <v>21668927311</v>
+      </c>
+      <c r="F4" s="2">
+        <v>31379530041</v>
+      </c>
+      <c r="G4" s="2">
+        <v>89865876042</v>
+      </c>
+      <c r="H4" s="2">
+        <v>195563714485</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>